<commit_message>
Write output file,  implementing DFA Tables,  tests
</commit_message>
<xml_diff>
--- a/Documentation/COMP-P2_worksheet.xlsx
+++ b/Documentation/COMP-P2_worksheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t xml:space="preserve">Color notation in the worksheet</t>
   </si>
@@ -154,16 +154,25 @@
     <t xml:space="preserve">Structure of the program</t>
   </si>
   <si>
+    <t xml:space="preserve">MA, AS</t>
+  </si>
+  <si>
     <t xml:space="preserve">The report</t>
   </si>
   <si>
     <t xml:space="preserve">Code and implementation (60%)</t>
   </si>
   <si>
+    <t xml:space="preserve">AS</t>
+  </si>
+  <si>
     <t xml:space="preserve">II</t>
   </si>
   <si>
     <t xml:space="preserve">Read in the input file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA</t>
   </si>
   <si>
     <t xml:space="preserve">Token List (in memory)</t>
@@ -598,7 +607,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="102.43"/>
@@ -727,13 +736,13 @@
   <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="3.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="28.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="28.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="5.85"/>
@@ -871,7 +880,9 @@
       <c r="B10" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="D10" s="23" t="s">
         <v>26</v>
       </c>
@@ -884,7 +895,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="23" t="s">
@@ -899,7 +910,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -914,9 +925,11 @@
       <c r="B13" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="22" t="s">
+        <v>34</v>
+      </c>
       <c r="D13" s="23" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="24"/>
@@ -927,11 +940,13 @@
         <v>14</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="22"/>
+        <v>36</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="D14" s="23" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="24"/>
@@ -942,7 +957,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="23" t="s">
@@ -957,9 +972,11 @@
         <v>16</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="22"/>
+        <v>39</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>34</v>
+      </c>
       <c r="D16" s="23" t="s">
         <v>28</v>
       </c>
@@ -972,7 +989,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="23" t="s">
@@ -991,7 +1008,7 @@
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="23" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="24"/>
@@ -1017,11 +1034,13 @@
         <v>20</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="22"/>
+        <v>41</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="D20" s="23" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="24"/>
@@ -1032,11 +1051,13 @@
         <v>21</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="22"/>
+        <v>42</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="D21" s="23" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="24"/>
@@ -1058,7 +1079,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
@@ -1074,7 +1095,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
@@ -1083,18 +1104,18 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="27" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="30" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1102,7 +1123,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="31" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C31" s="31"/>
       <c r="D31" s="31"/>

</xml_diff>

<commit_message>
Table fix, fill functions added, DFAs constructed, updated excel
</commit_message>
<xml_diff>
--- a/Documentation/COMP-P2_worksheet.xlsx
+++ b/Documentation/COMP-P2_worksheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t xml:space="preserve">Color notation in the worksheet</t>
   </si>
@@ -166,22 +166,25 @@
     <t xml:space="preserve">AS</t>
   </si>
   <si>
+    <t xml:space="preserve">FI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read in the input file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA</t>
+  </si>
+  <si>
     <t xml:space="preserve">II</t>
   </si>
   <si>
-    <t xml:space="preserve">Read in the input file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Token List (in memory)</t>
   </si>
   <si>
     <t xml:space="preserve">Create output file /release</t>
   </si>
   <si>
-    <t xml:space="preserve">AS, JV</t>
+    <t xml:space="preserve">JV</t>
   </si>
   <si>
     <t xml:space="preserve">Debug option of output</t>
@@ -610,7 +613,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="102.42"/>
@@ -722,8 +725,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -738,11 +741,11 @@
   </sheetPr>
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="3.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="28.3"/>
@@ -949,7 +952,7 @@
         <v>37</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="24"/>
@@ -960,7 +963,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="23" t="s">
@@ -975,10 +978,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>28</v>
@@ -992,7 +995,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="23" t="s">
@@ -1011,7 +1014,7 @@
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="23" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="24"/>
@@ -1037,13 +1040,13 @@
         <v>20</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="24"/>
@@ -1054,13 +1057,13 @@
         <v>21</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="24"/>
@@ -1082,7 +1085,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
@@ -1098,7 +1101,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
@@ -1107,18 +1110,18 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1126,7 +1129,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C31" s="31"/>
       <c r="D31" s="31"/>
@@ -1514,8 +1517,8 @@
     <mergeCell ref="B78:F78"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
-  <pageMargins left="0.236111111111111" right="0.236111111111111" top="0.157638888888889" bottom="0.157638888888889" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.236111111111111" right="0.236111111111111" top="0.157638888888889" bottom="0.157638888888889" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>